<commit_message>
Separacion bases de datos
Se añadieron nuevas variables y se separaron los datos en 3 bases de datos, 2012-2016, 2017-01,2018
</commit_message>
<xml_diff>
--- a/Archivos/ICC.xlsx
+++ b/Archivos/ICC.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jhonier\Desktop\TAE trabajo4\series usadas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jhonier\Documents\GitHub\TrabajoTAE4\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C9F008-248B-43E7-8F55-532B7D6D46E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117EE3F1-C9F6-4B23-8A7B-64B5A47E8AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{62BF19AA-684C-4C49-9006-7322F9D41145}"/>
   </bookViews>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{886F484C-EBE9-4379-AE6F-15924136B90E}">
-  <dimension ref="A1:D203"/>
+  <dimension ref="A1:D207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
+      <selection activeCell="D207" sqref="D207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3247,6 +3247,62 @@
         <v>-2.5</v>
       </c>
     </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="2">
+        <v>43344</v>
+      </c>
+      <c r="B204">
+        <v>-0.7</v>
+      </c>
+      <c r="C204">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D204">
+        <v>-9.4</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" s="2">
+        <v>43374</v>
+      </c>
+      <c r="B205">
+        <v>-1.3</v>
+      </c>
+      <c r="C205">
+        <v>3.9</v>
+      </c>
+      <c r="D205">
+        <v>-9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="2">
+        <v>43405</v>
+      </c>
+      <c r="B206">
+        <v>-19.600000000000001</v>
+      </c>
+      <c r="C206">
+        <v>-23.7</v>
+      </c>
+      <c r="D206">
+        <v>-13.5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="2">
+        <v>43435</v>
+      </c>
+      <c r="B207">
+        <v>-8.3000000000000007</v>
+      </c>
+      <c r="C207">
+        <v>-11.1</v>
+      </c>
+      <c r="D207">
+        <v>-4.0999999999999996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>